<commit_message>
correction template risk indicators
</commit_message>
<xml_diff>
--- a/uncertainty_models/UMCRF_I1.xlsx
+++ b/uncertainty_models/UMCRF_I1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\uncertainty_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7DB7CF-CE93-411E-9CE7-1BF8C82AFD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041CDA67-7645-4D08-A3E6-6CF487D616C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,34 +736,34 @@
         <v>0</v>
       </c>
       <c r="G2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="H2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="I2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="J2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="K2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="L2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="M2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="N2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="O2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="P2" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="Q2" s="6">
         <v>-0.5</v>
@@ -810,34 +810,34 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="H3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="I3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="J3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="K3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="L3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="M3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="N3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="O3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="P3" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="Q3" s="4">
         <v>-0.1</v>
@@ -884,34 +884,34 @@
         <v>0</v>
       </c>
       <c r="G4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="I4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="J4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="L4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="M4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="N4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="O4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="P4" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="Q4" s="4">
         <v>0.1</v>
@@ -958,34 +958,34 @@
         <v>0</v>
       </c>
       <c r="G5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="H5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="I5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="J5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="K5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="L5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="M5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="N5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="O5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="P5" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="Q5" s="15">
         <v>0.5</v>
@@ -1180,34 +1180,34 @@
         <v>0</v>
       </c>
       <c r="G8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="H8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="I8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="J8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="K8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="L8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="M8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="N8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="O8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="P8" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="Q8" s="6">
         <v>-0.5</v>
@@ -1254,34 +1254,34 @@
         <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="H9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="I9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="J9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="K9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="L9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="M9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="N9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="O9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="P9" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="Q9" s="4">
         <v>-0.1</v>
@@ -1328,34 +1328,34 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="J10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="K10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="L10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="M10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="N10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="O10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="P10" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="Q10" s="4">
         <v>0.1</v>
@@ -1402,34 +1402,34 @@
         <v>0</v>
       </c>
       <c r="G11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="H11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="I11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="J11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="K11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="L11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="M11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="N11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="O11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="P11" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="Q11" s="15">
         <v>0.5</v>
@@ -1624,34 +1624,34 @@
         <v>0</v>
       </c>
       <c r="G14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="H14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="I14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="J14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="K14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="L14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="M14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="N14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="O14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="P14" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="Q14" s="6">
         <v>-0.5</v>
@@ -1698,34 +1698,34 @@
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="H15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="I15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="J15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="K15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="L15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="M15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="N15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="O15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="P15" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="Q15" s="4">
         <v>-0.1</v>
@@ -1772,34 +1772,34 @@
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="H16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="I16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="J16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="K16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="L16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="M16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="N16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="O16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="P16" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="Q16" s="4">
         <v>0.1</v>
@@ -1846,34 +1846,34 @@
         <v>0</v>
       </c>
       <c r="G17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="H17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="I17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="J17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="K17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="L17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="M17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="N17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="O17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="P17" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="Q17" s="15">
         <v>0.5</v>
@@ -2068,34 +2068,34 @@
         <v>0</v>
       </c>
       <c r="G20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="H20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="I20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="J20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="K20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="L20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="M20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="N20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="O20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="P20" s="6">
-        <v>-0.1</v>
+        <v>-0.8</v>
       </c>
       <c r="Q20" s="6">
         <v>-0.5</v>
@@ -2142,34 +2142,34 @@
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="H21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="I21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="J21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="K21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="L21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="M21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="N21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="O21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="P21" s="4">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="Q21" s="4">
         <v>-0.1</v>
@@ -2216,34 +2216,34 @@
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="H22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="I22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="J22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="K22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="L22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="M22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="N22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="O22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="P22" s="4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="Q22" s="4">
         <v>0.1</v>
@@ -2290,34 +2290,34 @@
         <v>0</v>
       </c>
       <c r="G23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="H23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="I23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="J23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="K23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="L23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="M23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="N23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="O23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="P23" s="15">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="Q23" s="15">
         <v>0.5</v>

</xml_diff>